<commit_message>
updating table to make it more balanced
</commit_message>
<xml_diff>
--- a/Pontuação do jogo.xlsx
+++ b/Pontuação do jogo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gmv0-my.sharepoint.com/personal/dtms_gmv_com/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welli\Documents\0-2024\LP1\p1\2024ProjectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="423" documentId="14_{B4FD7E5B-05F8-4056-B834-C8B8621E6A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6524F9-B372-4B68-B786-771425D4147D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92CDD95-451A-4257-B018-05E66DE4FA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="390" windowWidth="23010" windowHeight="11925" xr2:uid="{A73730A3-D604-4BE2-95F6-5012C45723EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A73730A3-D604-4BE2-95F6-5012C45723EC}"/>
   </bookViews>
   <sheets>
     <sheet name="PedraPapelTesoura v2" sheetId="4" r:id="rId1"/>
@@ -402,7 +402,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF1F2328"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -567,32 +592,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89FC2FB7-892A-4401-AC78-9FF999F7C41D}" name="Table13" displayName="Table13" ref="A15:M28" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89FC2FB7-892A-4401-AC78-9FF999F7C41D}" name="Table13" displayName="Table13" ref="A15:M29" totalsRowCount="1" headerRowDxfId="2">
   <autoFilter ref="A15:M28" xr:uid="{3B35A3B8-EE56-441C-B388-8F841C446906}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AA951C0C-1CF4-4FFF-8E2C-550F38BFB339}" name="Column1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7A2D6FAF-C2F7-4A8F-8048-F82FD9157BA5}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{E9507762-EE9B-471F-A2E3-0B33E4EA00EE}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{6AFF9944-B162-4424-B29D-94C73D9FCF76}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{9CE5C747-306E-4E37-AB7A-36FE49EEF6B5}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{CD25C3DD-4E06-49FE-AC73-7B441C509F83}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{8E4789DA-B4E9-4EA0-84CF-775043E82886}" name="Column7"/>
-    <tableColumn id="8" xr3:uid="{C8CB16B8-D24F-40F9-98C2-6A04262E374A}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{4B2B57DB-901D-42B6-A0EF-6A728D182AB7}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{E6E915BE-FB21-4832-A3EC-91ED79699115}" name="Column10"/>
-    <tableColumn id="14" xr3:uid="{AE929358-3659-4FF5-8236-D589A8E14F8B}" name="Column102"/>
-    <tableColumn id="11" xr3:uid="{5F194D0E-A00F-4631-B43F-EBB86082D79C}" name="Column11"/>
-    <tableColumn id="12" xr3:uid="{71E9CA49-0BD6-4685-BC05-1D78076CDC45}" name="Column12"/>
+    <tableColumn id="1" xr3:uid="{AA951C0C-1CF4-4FFF-8E2C-550F38BFB339}" name="Column1" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{7A2D6FAF-C2F7-4A8F-8048-F82FD9157BA5}" name="Column2" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(B17:B26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E9507762-EE9B-471F-A2E3-0B33E4EA00EE}" name="Column3" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(C17:C26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{6AFF9944-B162-4424-B29D-94C73D9FCF76}" name="Column4" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(D17:D26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{9CE5C747-306E-4E37-AB7A-36FE49EEF6B5}" name="Column5" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(E17:E26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{CD25C3DD-4E06-49FE-AC73-7B441C509F83}" name="Column6" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(F17:F26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{8E4789DA-B4E9-4EA0-84CF-775043E82886}" name="Column7" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(G17:G26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C8CB16B8-D24F-40F9-98C2-6A04262E374A}" name="Column8" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(H17:H26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{4B2B57DB-901D-42B6-A0EF-6A728D182AB7}" name="Column9" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(I17:I26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{E6E915BE-FB21-4832-A3EC-91ED79699115}" name="Column10" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(J17:J26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{AE929358-3659-4FF5-8236-D589A8E14F8B}" name="Column102" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(K17:K26)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{5F194D0E-A00F-4631-B43F-EBB86082D79C}" name="Column11" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(L17:L28)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{71E9CA49-0BD6-4685-BC05-1D78076CDC45}" name="Column12" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(M17:M28)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{488B84C2-9E81-4C15-9753-F2FC4E16A511}" name="Table134" displayName="Table134" ref="A90:M103" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{488B84C2-9E81-4C15-9753-F2FC4E16A511}" name="Table134" displayName="Table134" ref="A90:M103" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A90:M103" xr:uid="{488B84C2-9E81-4C15-9753-F2FC4E16A511}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{B90777BD-1881-4E2F-A5B9-AC010FBF058D}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B90777BD-1881-4E2F-A5B9-AC010FBF058D}" name="Column1" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{0C2D42CB-8713-4B45-91AF-4366562598B6}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{E44CC5B7-C082-4010-B02E-D56577AD1CF6}" name="Column3"/>
     <tableColumn id="4" xr3:uid="{738E8E54-D824-4EB0-809C-3D88E427E6E9}" name="Column4"/>
@@ -611,10 +660,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B35A3B8-EE56-441C-B388-8F841C446906}" name="Table1" displayName="Table1" ref="A15:M28" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B35A3B8-EE56-441C-B388-8F841C446906}" name="Table1" displayName="Table1" ref="A15:M28" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A15:M28" xr:uid="{3B35A3B8-EE56-441C-B388-8F841C446906}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{17319E0E-CE45-423C-A64C-38F28A2F735C}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{17319E0E-CE45-423C-A64C-38F28A2F735C}" name="Column1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{5EE1A0F1-FBF7-4DDC-806E-1D55E2DBDEE1}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{576F3BB1-EC9C-4333-9BAD-47B8824FB804}" name="Column3"/>
     <tableColumn id="4" xr3:uid="{533DCB86-3429-42B9-8769-9383C741608C}" name="Column4"/>
@@ -633,9 +682,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -673,7 +722,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -779,7 +828,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -921,7 +970,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -931,14 +980,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555E6FC2-07FF-4BF5-9FD7-418781A69E93}">
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="13" width="15.5703125" customWidth="1"/>
+    <col min="1" max="13" width="15.5703125" customWidth="1"/>
     <col min="14" max="14" width="12.5703125" customWidth="1"/>
     <col min="25" max="25" width="11.140625" customWidth="1"/>
   </cols>
@@ -1178,7 +1226,7 @@
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
     </row>
-    <row r="15" spans="1:26" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1299,35 +1347,27 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>+Table13[[#This Row],[Column2]]+4</f>
         <v>4</v>
       </c>
       <c r="D17">
-        <f>+Table13[[#This Row],[Column3]]+4</f>
         <v>8</v>
       </c>
       <c r="E17">
-        <f>+Table13[[#This Row],[Column4]]+4</f>
         <v>12</v>
       </c>
       <c r="F17">
-        <f>+Table13[[#This Row],[Column5]]+4</f>
         <v>16</v>
       </c>
       <c r="G17">
-        <f>+Table13[[#This Row],[Column6]]+4</f>
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="H17">
-        <f>+Table13[[#This Row],[Column7]]-36</f>
         <v>-16</v>
       </c>
       <c r="I17">
-        <f>+Table13[[#This Row],[Column8]]+4</f>
-        <v>-12</v>
+        <v>12</v>
       </c>
       <c r="J17">
-        <f>+Table13[[#This Row],[Column9]]+4</f>
         <v>-8</v>
       </c>
       <c r="K17">
@@ -1337,7 +1377,11 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="N17">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
+        <v>4</v>
       </c>
       <c r="O17" s="12" t="s">
         <v>13</v>
@@ -1364,7 +1408,7 @@
       </c>
       <c r="U17" s="13">
         <f>+Table13[[#This Row],[Column7]]</f>
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="V17" s="13">
         <f>+Table13[[#This Row],[Column8]]</f>
@@ -1372,7 +1416,7 @@
       </c>
       <c r="W17" s="13">
         <f>+Table13[[#This Row],[Column9]]</f>
-        <v>-12</v>
+        <v>12</v>
       </c>
       <c r="X17" s="13">
         <f>+Table13[[#This Row],[Column10]]</f>
@@ -1391,48 +1435,45 @@
         <v>14</v>
       </c>
       <c r="B18">
-        <f>+B17-4</f>
+        <f>-C17</f>
         <v>-4</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18">
-        <f>+Table13[[#This Row],[Column3]]+4</f>
         <v>4</v>
       </c>
       <c r="E18">
-        <f>+Table13[[#This Row],[Column4]]+4</f>
         <v>8</v>
       </c>
       <c r="F18">
-        <f>+Table13[[#This Row],[Column5]]+4</f>
         <v>12</v>
       </c>
       <c r="G18">
-        <f>+Table13[[#This Row],[Column6]]+4</f>
         <v>16</v>
       </c>
       <c r="H18">
-        <f>+Table13[[#This Row],[Column7]]+4</f>
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="I18">
-        <f>+Table13[[#This Row],[Column8]]-36</f>
         <v>-16</v>
       </c>
       <c r="J18">
-        <f>+Table13[[#This Row],[Column9]]+4</f>
         <v>-12</v>
       </c>
       <c r="K18">
-        <v>-8</v>
+        <v>16</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="N18">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
+        <v>4</v>
       </c>
       <c r="O18" s="12" t="s">
         <v>4</v>
@@ -1463,7 +1504,7 @@
       </c>
       <c r="V18" s="13">
         <f>+Table13[[#This Row],[Column8]]</f>
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="W18" s="13">
         <f>+Table13[[#This Row],[Column9]]</f>
@@ -1486,46 +1527,46 @@
         <v>15</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:H25" si="0">+B18-4</f>
+        <f>-D17</f>
         <v>-8</v>
       </c>
       <c r="C19">
-        <f>+C18-4</f>
+        <f>-D18</f>
         <v>-4</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19">
-        <f>+E18-4</f>
         <v>4</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:J24" si="1">+F18-4</f>
         <v>8</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="I19">
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="J19">
         <v>-16</v>
       </c>
       <c r="K19">
-        <v>-12</v>
+        <v>12</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="N19">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
+        <v>4</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>16</v>
@@ -1560,7 +1601,7 @@
       </c>
       <c r="W19" s="13">
         <f>+Table13[[#This Row],[Column9]]</f>
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="X19" s="13">
         <f>+Table13[[#This Row],[Column10]]</f>
@@ -1579,34 +1620,30 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f>-E17</f>
         <v>-12</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f>-E18</f>
         <v>-8</v>
       </c>
       <c r="D20">
-        <f>+D19-4</f>
+        <f>-E19</f>
         <v>-4</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I20">
-        <f>+I19-4</f>
         <v>16</v>
       </c>
       <c r="J20">
@@ -1619,7 +1656,11 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="N20">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
+        <v>4</v>
       </c>
       <c r="O20" s="12" t="s">
         <v>18</v>
@@ -1646,7 +1687,7 @@
       </c>
       <c r="U20" s="13">
         <f>+Table13[[#This Row],[Column7]]</f>
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="V20" s="13">
         <f>+Table13[[#This Row],[Column8]]</f>
@@ -1673,38 +1714,34 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f>-F17</f>
         <v>-16</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f>-F18</f>
         <v>-12</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f>-F19</f>
         <v>-8</v>
       </c>
       <c r="E21">
-        <f>+E20-4</f>
+        <f>-F20</f>
         <v>-4</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="J21">
-        <f>+J20-4</f>
         <v>16</v>
       </c>
       <c r="K21">
@@ -1714,7 +1751,11 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="N21">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
+        <v>4</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>20</v>
@@ -1745,7 +1786,7 @@
       </c>
       <c r="V21" s="13">
         <f>+Table13[[#This Row],[Column8]]</f>
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="W21" s="13">
         <f>+Table13[[#This Row],[Column9]]</f>
@@ -1768,47 +1809,49 @@
         <v>21</v>
       </c>
       <c r="B22">
+        <f>-G17</f>
         <v>20</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f>-G18</f>
         <v>-16</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f>-G19</f>
         <v>-12</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>-8</v>
+        <f>-G20</f>
+        <v>8</v>
       </c>
       <c r="F22">
-        <f>+F21-4</f>
+        <f>-G21</f>
         <v>-4</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J22">
-        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="K22">
-        <v>16</v>
+        <v>-16</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="N22">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
+        <v>4</v>
       </c>
       <c r="O22" s="12" t="s">
         <v>22</v>
@@ -1827,7 +1870,7 @@
       </c>
       <c r="S22" s="13">
         <f>+Table13[[#This Row],[Column5]]</f>
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="T22" s="13">
         <f>+Table13[[#This Row],[Column6]]</f>
@@ -1862,47 +1905,50 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <f>+B22-4</f>
+        <f>-H17</f>
         <v>16</v>
       </c>
       <c r="C23">
+        <f>-H18</f>
         <v>20</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f>-H19</f>
         <v>-16</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f>-H20</f>
         <v>-12</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f>-H21</f>
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <f>-H22</f>
+        <v>-4</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23">
         <v>-8</v>
       </c>
-      <c r="G23">
-        <f>+G22-4</f>
+      <c r="J23">
         <v>-4</v>
       </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
       <c r="K23">
-        <v>12</v>
+        <v>-8</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="N23">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
+        <v>-8</v>
       </c>
       <c r="O23" s="12" t="s">
         <v>24</v>
@@ -1925,7 +1971,7 @@
       </c>
       <c r="T23" s="13">
         <f>+Table13[[#This Row],[Column6]]</f>
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="U23" s="13">
         <f>+Table13[[#This Row],[Column7]]</f>
@@ -1937,11 +1983,11 @@
       </c>
       <c r="W23" s="13">
         <f>+Table13[[#This Row],[Column9]]</f>
-        <v>4</v>
+        <v>-8</v>
       </c>
       <c r="X23" s="13">
         <f>+Table13[[#This Row],[Column10]]</f>
-        <v>8</v>
+        <v>-4</v>
       </c>
       <c r="Y23" s="13">
         <f>+Table13[[#This Row],[Column11]]</f>
@@ -1956,54 +2002,58 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:C25" si="2">+B23-4</f>
-        <v>12</v>
+        <f>-I17</f>
+        <v>-12</v>
       </c>
       <c r="C24">
-        <f>+C23-4</f>
+        <f>-I18</f>
         <v>16</v>
       </c>
       <c r="D24">
+        <f>-I19</f>
         <v>20</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f>-I20</f>
         <v>-16</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f>-I21</f>
         <v>-12</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
+        <f>-I22</f>
         <v>-8</v>
       </c>
       <c r="H24">
-        <f>+H23-4</f>
-        <v>-4</v>
+        <f>-I23</f>
+        <v>8</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
       </c>
       <c r="J24">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K24">
-        <v>8</v>
+        <v>-20</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="N24">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
+        <v>-8</v>
       </c>
       <c r="O24" s="12" t="s">
         <v>26</v>
       </c>
       <c r="P24" s="13">
         <f>+Table13[[#This Row],[Column2]]</f>
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="Q24" s="13">
         <f>+Table13[[#This Row],[Column3]]</f>
@@ -2027,7 +2077,7 @@
       </c>
       <c r="V24" s="13">
         <f>+Table13[[#This Row],[Column8]]</f>
-        <v>-4</v>
+        <v>8</v>
       </c>
       <c r="W24" s="13">
         <f>+Table13[[#This Row],[Column9]]</f>
@@ -2035,7 +2085,7 @@
       </c>
       <c r="X24" s="13">
         <f>+Table13[[#This Row],[Column10]]</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="Y24" s="13">
         <f>+Table13[[#This Row],[Column11]]</f>
@@ -2045,52 +2095,57 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B25">
-        <f t="shared" si="2"/>
+        <f>-J17</f>
         <v>8</v>
       </c>
       <c r="C25">
-        <f t="shared" si="2"/>
+        <f>-J18</f>
         <v>12</v>
       </c>
       <c r="D25">
-        <f>+D24-4</f>
+        <f>-J19</f>
         <v>16</v>
       </c>
       <c r="E25">
-        <v>20</v>
+        <f>-J20</f>
+        <v>-20</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f>-J21</f>
         <v>-16</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
+        <f>-J22</f>
         <v>-12</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
-        <v>-8</v>
+        <f>-J23</f>
+        <v>4</v>
       </c>
       <c r="I25">
-        <f>+I24-4</f>
+        <f>-J24</f>
+        <v>-16</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>20</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>20</v>
+      </c>
+      <c r="N25">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
         <v>-4</v>
-      </c>
-      <c r="J25" s="1">
-        <v>0</v>
-      </c>
-      <c r="K25" s="1">
-        <v>4</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
       </c>
       <c r="O25" s="12" t="s">
         <v>28</v>
@@ -2109,7 +2164,7 @@
       </c>
       <c r="S25" s="13">
         <f>+Table13[[#This Row],[Column5]]</f>
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="T25" s="13">
         <f>+Table13[[#This Row],[Column6]]</f>
@@ -2121,11 +2176,11 @@
       </c>
       <c r="V25" s="13">
         <f>+Table13[[#This Row],[Column8]]</f>
-        <v>-8</v>
+        <v>4</v>
       </c>
       <c r="W25" s="13">
         <f>+Table13[[#This Row],[Column9]]</f>
-        <v>-4</v>
+        <v>-16</v>
       </c>
       <c r="X25" s="13">
         <f>+Table13[[#This Row],[Column10]]</f>
@@ -2144,40 +2199,52 @@
         <v>48</v>
       </c>
       <c r="B26">
+        <f>-K17</f>
         <v>4</v>
       </c>
       <c r="C26">
+        <f>-K18</f>
+        <v>-16</v>
+      </c>
+      <c r="D26">
+        <f>-K19</f>
+        <v>-12</v>
+      </c>
+      <c r="E26">
+        <f>-K20</f>
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <f>-K21</f>
+        <v>-20</v>
+      </c>
+      <c r="G26">
+        <f>-K22</f>
+        <v>16</v>
+      </c>
+      <c r="H26">
+        <f>-K23</f>
         <v>8</v>
       </c>
-      <c r="D26">
-        <v>12</v>
-      </c>
-      <c r="E26">
-        <v>16</v>
-      </c>
-      <c r="F26">
-        <v>20</v>
-      </c>
-      <c r="G26">
-        <v>-16</v>
-      </c>
-      <c r="H26">
-        <v>-12</v>
-      </c>
       <c r="I26">
-        <v>-8</v>
+        <f>-K24</f>
+        <v>20</v>
       </c>
       <c r="J26" s="1">
+        <v>-20</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>20</v>
+      </c>
+      <c r="N26">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column102]])</f>
         <v>-4</v>
-      </c>
-      <c r="K26" s="1">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
       </c>
       <c r="O26" s="12" t="s">
         <v>30</v>
@@ -2188,11 +2255,11 @@
       </c>
       <c r="Q26" s="13">
         <f>+Table13[[#This Row],[Column3]]</f>
-        <v>8</v>
+        <v>-16</v>
       </c>
       <c r="R26" s="13">
         <f>+Table13[[#This Row],[Column4]]</f>
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="S26" s="13">
         <f>+Table13[[#This Row],[Column5]]</f>
@@ -2200,23 +2267,23 @@
       </c>
       <c r="T26" s="13">
         <f>+Table13[[#This Row],[Column6]]</f>
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="U26" s="13">
         <f>+Table13[[#This Row],[Column7]]</f>
-        <v>-16</v>
+        <v>16</v>
       </c>
       <c r="V26" s="13">
         <f>+Table13[[#This Row],[Column8]]</f>
-        <v>-12</v>
+        <v>8</v>
       </c>
       <c r="W26" s="13">
         <f>+Table13[[#This Row],[Column9]]</f>
-        <v>-8</v>
+        <v>20</v>
       </c>
       <c r="X26" s="13">
         <f>+Table13[[#This Row],[Column10]]</f>
-        <v>-4</v>
+        <v>-20</v>
       </c>
       <c r="Y26" s="13">
         <f>+Table13[[#This Row],[Column11]]</f>
@@ -2231,6 +2298,7 @@
         <v>29</v>
       </c>
       <c r="B27">
+        <f>-L17</f>
         <v>0</v>
       </c>
       <c r="C27">
@@ -2249,6 +2317,7 @@
         <v>0</v>
       </c>
       <c r="H27">
+        <f>-L24</f>
         <v>0</v>
       </c>
       <c r="I27">
@@ -2264,6 +2333,10 @@
         <v>0</v>
       </c>
       <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column12]])</f>
         <v>0</v>
       </c>
       <c r="O27" s="12" t="s">
@@ -2308,34 +2381,41 @@
         <v>47</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <f>-M17</f>
+        <v>-20</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <f>-M18</f>
+        <v>-20</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <f>-M19</f>
+        <v>-20</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <f>-M20</f>
+        <v>-20</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <f>-M21</f>
+        <v>-20</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <f>-M22</f>
+        <v>-20</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <f>-M24</f>
+        <v>-20</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="L28" s="1">
         <v>0</v>
@@ -2343,8 +2423,62 @@
       <c r="M28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="N28">
+        <f>SUM(Table13[[#This Row],[Column2]:[Column12]])</f>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29">
+        <f t="shared" ref="B29:I29" si="0">SUM(B17:B26)</f>
+        <v>-4</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <f>SUM(I17:I26)</f>
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <f>SUM(J17:J26)</f>
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <f>SUM(K17:K26)</f>
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <f>SUM(L17:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f>SUM(M17:M28)</f>
+        <v>200</v>
+      </c>
+    </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>0</v>
@@ -2433,11 +2567,11 @@
         <v>13</v>
       </c>
       <c r="B34">
-        <f t="shared" ref="B34:B41" si="3">IF(A34="D",B33+100,B33-25)</f>
+        <f t="shared" ref="B34:B41" si="1">IF(A34="D",B33+100,B33-25)</f>
         <v>950</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C41" si="4">IF(A34="D", C33+100, IF(D34&lt;0, C33+D34, C33))</f>
+        <f t="shared" ref="C34:C41" si="2">IF(A34="D", C33+100, IF(D34&lt;0, C33+D34, C33))</f>
         <v>1000</v>
       </c>
       <c r="D34" s="15">
@@ -2448,11 +2582,11 @@
         <v>20</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F41" si="5">IF(E34="D", F33+100, IF(D34&gt;0, F33-D34, F33))</f>
+        <f t="shared" ref="F34:F41" si="3">IF(E34="D", F33+100, IF(D34&gt;0, F33-D34, F33))</f>
         <v>980</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G34:G41" si="6">IF(D34 &gt;0, G33-D34, G33)</f>
+        <f t="shared" ref="G34:G41" si="4">IF(D34 &gt;0, G33-D34, G33)</f>
         <v>980</v>
       </c>
     </row>
@@ -2461,27 +2595,27 @@
         <v>13</v>
       </c>
       <c r="B35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>925</v>
       </c>
       <c r="C35">
-        <f t="shared" si="4"/>
-        <v>1000</v>
+        <f t="shared" si="2"/>
+        <v>980</v>
       </c>
       <c r="D35" s="15">
-        <f t="shared" ref="D35:D41" si="7">INDEX($P$17:$Y$26,MATCH(A35,$O$17:$O$26,0),MATCH(E35,$P$16:$Y$16,0))</f>
-        <v>20</v>
+        <f t="shared" ref="D35:D41" si="5">INDEX($P$17:$Y$26,MATCH(A35,$O$17:$O$26,0),MATCH(E35,$P$16:$Y$16,0))</f>
+        <v>-20</v>
       </c>
       <c r="E35" t="s">
         <v>22</v>
       </c>
       <c r="F35">
-        <f t="shared" si="5"/>
-        <v>960</v>
+        <f t="shared" si="3"/>
+        <v>980</v>
       </c>
       <c r="G35">
-        <f t="shared" si="6"/>
-        <v>960</v>
+        <f t="shared" si="4"/>
+        <v>980</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2489,27 +2623,27 @@
         <v>13</v>
       </c>
       <c r="B36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>900</v>
       </c>
       <c r="C36">
-        <f t="shared" si="4"/>
-        <v>1000</v>
+        <f t="shared" si="2"/>
+        <v>960</v>
       </c>
       <c r="D36" s="15">
-        <f t="shared" si="7"/>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>-20</v>
       </c>
       <c r="E36" t="s">
         <v>22</v>
       </c>
       <c r="F36">
-        <f t="shared" si="5"/>
-        <v>940</v>
+        <f t="shared" si="3"/>
+        <v>980</v>
       </c>
       <c r="G36">
-        <f t="shared" si="6"/>
-        <v>940</v>
+        <f t="shared" si="4"/>
+        <v>980</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2517,27 +2651,27 @@
         <v>28</v>
       </c>
       <c r="B37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>875</v>
       </c>
       <c r="C37">
-        <f t="shared" si="4"/>
-        <v>1000</v>
+        <f t="shared" si="2"/>
+        <v>960</v>
       </c>
       <c r="D37" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E37" t="s">
         <v>28</v>
       </c>
       <c r="F37">
-        <f t="shared" si="5"/>
-        <v>940</v>
+        <f t="shared" si="3"/>
+        <v>980</v>
       </c>
       <c r="G37">
-        <f t="shared" si="6"/>
-        <v>940</v>
+        <f t="shared" si="4"/>
+        <v>980</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2545,27 +2679,27 @@
         <v>30</v>
       </c>
       <c r="B38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>975</v>
       </c>
       <c r="C38">
-        <f t="shared" si="4"/>
-        <v>1100</v>
+        <f t="shared" si="2"/>
+        <v>1060</v>
       </c>
       <c r="D38" s="15">
-        <f t="shared" si="7"/>
-        <v>-16</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
         <v>22</v>
       </c>
       <c r="F38">
         <f>IF(E38="D", F37+100, IF(D38&gt;0, F37-D38, F37))</f>
-        <v>940</v>
+        <v>964</v>
       </c>
       <c r="G38">
-        <f t="shared" si="6"/>
-        <v>940</v>
+        <f t="shared" si="4"/>
+        <v>964</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2573,27 +2707,27 @@
         <v>22</v>
       </c>
       <c r="B39">
+        <f t="shared" si="1"/>
+        <v>950</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>1056</v>
+      </c>
+      <c r="D39" s="15">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39">
         <f t="shared" si="3"/>
-        <v>950</v>
-      </c>
-      <c r="C39">
+        <v>964</v>
+      </c>
+      <c r="G39">
         <f t="shared" si="4"/>
-        <v>1096</v>
-      </c>
-      <c r="D39" s="15">
-        <f t="shared" si="7"/>
-        <v>-4</v>
-      </c>
-      <c r="E39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="5"/>
-        <v>940</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="6"/>
-        <v>940</v>
+        <v>964</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2601,27 +2735,27 @@
         <v>20</v>
       </c>
       <c r="B40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>925</v>
       </c>
       <c r="C40">
-        <f t="shared" si="4"/>
-        <v>1096</v>
+        <f t="shared" si="2"/>
+        <v>1056</v>
       </c>
       <c r="D40" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E40" t="s">
         <v>30</v>
       </c>
       <c r="F40">
-        <f t="shared" si="5"/>
-        <v>1040</v>
+        <f t="shared" si="3"/>
+        <v>1064</v>
       </c>
       <c r="G40">
-        <f t="shared" si="6"/>
-        <v>940</v>
+        <f t="shared" si="4"/>
+        <v>964</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2629,27 +2763,27 @@
         <v>16</v>
       </c>
       <c r="B41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>900</v>
       </c>
       <c r="C41">
-        <f t="shared" si="4"/>
-        <v>1096</v>
+        <f t="shared" si="2"/>
+        <v>1056</v>
       </c>
       <c r="D41" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="E41" t="s">
         <v>22</v>
       </c>
       <c r="F41">
-        <f t="shared" si="5"/>
-        <v>1028</v>
+        <f t="shared" si="3"/>
+        <v>1052</v>
       </c>
       <c r="G41">
-        <f t="shared" si="6"/>
-        <v>928</v>
+        <f t="shared" si="4"/>
+        <v>952</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2694,7 +2828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>12</v>
       </c>
@@ -2703,48 +2837,48 @@
         <v>0</v>
       </c>
       <c r="C46" s="13">
-        <f t="shared" ref="C46:K46" si="8">+C17*(3/4)</f>
+        <f t="shared" ref="C46:K46" si="6">+C17*(3/4)</f>
         <v>3</v>
       </c>
       <c r="D46" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="E46" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="F46" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="G46" s="13">
-        <f t="shared" si="8"/>
-        <v>15</v>
+        <f t="shared" si="6"/>
+        <v>-15</v>
       </c>
       <c r="H46" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>-12</v>
       </c>
       <c r="I46" s="13">
-        <f t="shared" si="8"/>
-        <v>-9</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="J46" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>-6</v>
       </c>
       <c r="K46" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>-3</v>
       </c>
       <c r="L46" s="13">
-        <f t="shared" ref="B46:M57" si="9">+L17</f>
+        <f t="shared" ref="B46:M57" si="7">+L17</f>
         <v>0</v>
       </c>
       <c r="M46" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -2752,52 +2886,52 @@
         <v>14</v>
       </c>
       <c r="B47" s="13">
-        <f t="shared" ref="B47:K55" si="10">+B18*(3/4)</f>
+        <f t="shared" ref="B47:K55" si="8">+B18*(3/4)</f>
         <v>-3</v>
       </c>
       <c r="C47" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D47" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="E47" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="F47" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="G47" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="H47" s="13">
-        <f t="shared" si="10"/>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>-15</v>
       </c>
       <c r="I47" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-12</v>
       </c>
       <c r="J47" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-9</v>
       </c>
       <c r="K47" s="13">
-        <f t="shared" si="10"/>
-        <v>-6</v>
+        <f t="shared" si="8"/>
+        <v>12</v>
       </c>
       <c r="L47" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M47" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -2805,52 +2939,52 @@
         <v>15</v>
       </c>
       <c r="B48" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-6</v>
       </c>
       <c r="C48" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-3</v>
       </c>
       <c r="D48" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E48" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="F48" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="G48" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="H48" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="I48" s="13">
-        <f t="shared" si="10"/>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>-15</v>
       </c>
       <c r="J48" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-12</v>
       </c>
       <c r="K48" s="13">
-        <f t="shared" si="10"/>
-        <v>-9</v>
+        <f t="shared" si="8"/>
+        <v>9</v>
       </c>
       <c r="L48" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M48" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -2858,52 +2992,52 @@
         <v>17</v>
       </c>
       <c r="B49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-9</v>
       </c>
       <c r="C49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-6</v>
       </c>
       <c r="D49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-3</v>
       </c>
       <c r="E49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="G49" s="13">
-        <f t="shared" si="10"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>-6</v>
       </c>
       <c r="H49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="I49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="J49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="K49" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-12</v>
       </c>
       <c r="L49" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M49" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -2911,52 +3045,52 @@
         <v>19</v>
       </c>
       <c r="B50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-12</v>
       </c>
       <c r="C50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-9</v>
       </c>
       <c r="D50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-6</v>
       </c>
       <c r="E50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-3</v>
       </c>
       <c r="F50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H50" s="13">
-        <f t="shared" si="10"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>-6</v>
       </c>
       <c r="I50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="J50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="K50" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="L50" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -2964,105 +3098,105 @@
         <v>21</v>
       </c>
       <c r="B51" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="C51" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-12</v>
       </c>
       <c r="D51" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-9</v>
       </c>
       <c r="E51" s="13">
-        <f t="shared" si="10"/>
-        <v>-6</v>
+        <f t="shared" si="8"/>
+        <v>6</v>
       </c>
       <c r="F51" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-3</v>
       </c>
       <c r="G51" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H51" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="I51" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="J51" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="K51" s="13">
-        <f t="shared" si="10"/>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>-12</v>
       </c>
       <c r="L51" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M51" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="C52" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D52" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-12</v>
       </c>
       <c r="E52" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-9</v>
       </c>
       <c r="F52" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="G52" s="13">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="H52" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="13">
+        <f t="shared" si="8"/>
         <v>-6</v>
       </c>
-      <c r="G52" s="13">
-        <f t="shared" si="10"/>
+      <c r="J52" s="13">
+        <f t="shared" si="8"/>
         <v>-3</v>
       </c>
-      <c r="H52" s="13">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I52" s="13">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="J52" s="13">
-        <f t="shared" si="10"/>
-        <v>6</v>
-      </c>
       <c r="K52" s="13">
-        <f t="shared" si="10"/>
-        <v>9</v>
+        <f t="shared" si="8"/>
+        <v>-6</v>
       </c>
       <c r="L52" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M52" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -3070,52 +3204,52 @@
         <v>25</v>
       </c>
       <c r="B53" s="13">
-        <f t="shared" si="10"/>
-        <v>9</v>
+        <f t="shared" si="8"/>
+        <v>-9</v>
       </c>
       <c r="C53" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="D53" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="E53" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-12</v>
       </c>
       <c r="F53" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-9</v>
       </c>
       <c r="G53" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>-6</v>
       </c>
       <c r="H53" s="13">
-        <f t="shared" si="10"/>
-        <v>-3</v>
+        <f t="shared" si="8"/>
+        <v>6</v>
       </c>
       <c r="I53" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J53" s="13">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f t="shared" si="8"/>
+        <v>12</v>
       </c>
       <c r="K53" s="13">
-        <f t="shared" si="10"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>-15</v>
       </c>
       <c r="L53" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M53" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
@@ -3123,52 +3257,52 @@
         <v>27</v>
       </c>
       <c r="B54" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="C54" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="D54" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="E54" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="F54" s="13">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="G54" s="13">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="H54" s="13">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="I54" s="13">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="J54" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="13">
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="F54" s="13">
-        <f t="shared" si="10"/>
-        <v>-12</v>
-      </c>
-      <c r="G54" s="13">
-        <f t="shared" si="10"/>
-        <v>-9</v>
-      </c>
-      <c r="H54" s="13">
-        <f t="shared" si="10"/>
-        <v>-6</v>
-      </c>
-      <c r="I54" s="13">
-        <f t="shared" si="10"/>
-        <v>-3</v>
-      </c>
-      <c r="J54" s="13">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K54" s="13">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
       <c r="L54" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M54" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -3176,52 +3310,52 @@
         <v>48</v>
       </c>
       <c r="B55" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="C55" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="D55" s="13">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="E55" s="13">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="F55" s="13">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="G55" s="13">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="H55" s="13">
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="D55" s="13">
-        <f t="shared" si="10"/>
-        <v>9</v>
-      </c>
-      <c r="E55" s="13">
-        <f t="shared" si="10"/>
-        <v>12</v>
-      </c>
-      <c r="F55" s="13">
-        <f t="shared" si="10"/>
+      <c r="I55" s="13">
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="G55" s="13">
-        <f t="shared" si="10"/>
-        <v>-12</v>
-      </c>
-      <c r="H55" s="13">
-        <f t="shared" si="10"/>
-        <v>-9</v>
-      </c>
-      <c r="I55" s="13">
-        <f t="shared" si="10"/>
-        <v>-6</v>
-      </c>
       <c r="J55" s="13">
-        <f t="shared" si="10"/>
-        <v>-3</v>
+        <f t="shared" si="8"/>
+        <v>-15</v>
       </c>
       <c r="K55" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L55" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M55" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -3229,51 +3363,51 @@
         <v>29</v>
       </c>
       <c r="B56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M56" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3282,51 +3416,51 @@
         <v>47</v>
       </c>
       <c r="B57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="C57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="D57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="E57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="F57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="G57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="H57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="I57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="J57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="K57" s="13">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-20</v>
       </c>
       <c r="L57" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M57" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3369,7 +3503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>12</v>
       </c>
@@ -3378,39 +3512,39 @@
         <v>0</v>
       </c>
       <c r="C60" s="16">
-        <f t="shared" ref="C60:K60" si="11">+C17/2</f>
+        <f t="shared" ref="C60:K60" si="9">+C17/2</f>
         <v>2</v>
       </c>
       <c r="D60" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="E60" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="F60" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="G60" s="16">
-        <f t="shared" si="11"/>
-        <v>10</v>
+        <f t="shared" si="9"/>
+        <v>-10</v>
       </c>
       <c r="H60" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-8</v>
       </c>
       <c r="I60" s="16">
-        <f t="shared" si="11"/>
-        <v>-6</v>
+        <f t="shared" si="9"/>
+        <v>6</v>
       </c>
       <c r="J60" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-4</v>
       </c>
       <c r="K60" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-2</v>
       </c>
       <c r="L60" s="16">
@@ -3425,44 +3559,44 @@
         <v>14</v>
       </c>
       <c r="B61" s="16">
-        <f t="shared" ref="B61:K69" si="12">+B18/2</f>
+        <f t="shared" ref="B61:K69" si="10">+B18/2</f>
         <v>-2</v>
       </c>
       <c r="C61" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D61" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="E61" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="F61" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="G61" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="H61" s="16">
-        <f t="shared" si="12"/>
-        <v>10</v>
+        <f t="shared" si="10"/>
+        <v>-10</v>
       </c>
       <c r="I61" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-8</v>
       </c>
       <c r="J61" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-6</v>
       </c>
       <c r="K61" s="16">
-        <f t="shared" si="12"/>
-        <v>-4</v>
+        <f t="shared" si="10"/>
+        <v>8</v>
       </c>
       <c r="L61" s="5">
         <v>0</v>
@@ -3476,44 +3610,44 @@
         <v>15</v>
       </c>
       <c r="B62" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-4</v>
       </c>
       <c r="C62" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="D62" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E62" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="F62" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="G62" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="H62" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="I62" s="16">
-        <f t="shared" si="12"/>
-        <v>10</v>
+        <f t="shared" si="10"/>
+        <v>-10</v>
       </c>
       <c r="J62" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-8</v>
       </c>
       <c r="K62" s="16">
-        <f t="shared" si="12"/>
-        <v>-6</v>
+        <f t="shared" si="10"/>
+        <v>6</v>
       </c>
       <c r="L62" s="16">
         <v>0</v>
@@ -3527,43 +3661,43 @@
         <v>17</v>
       </c>
       <c r="B63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-6</v>
       </c>
       <c r="C63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-4</v>
       </c>
       <c r="D63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="E63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="G63" s="16">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>-4</v>
       </c>
       <c r="H63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="I63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="J63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="K63" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-8</v>
       </c>
       <c r="L63" s="5">
@@ -3578,43 +3712,43 @@
         <v>19</v>
       </c>
       <c r="B64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-8</v>
       </c>
       <c r="C64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-6</v>
       </c>
       <c r="D64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-4</v>
       </c>
       <c r="E64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="F64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="H64" s="16">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>-4</v>
       </c>
       <c r="I64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="K64" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="L64" s="16">
@@ -3629,44 +3763,44 @@
         <v>21</v>
       </c>
       <c r="B65" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="C65" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-8</v>
       </c>
       <c r="D65" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-6</v>
       </c>
       <c r="E65" s="16">
-        <f t="shared" si="12"/>
-        <v>-4</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
       <c r="F65" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="G65" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H65" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I65" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="J65" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="K65" s="16">
-        <f t="shared" si="12"/>
-        <v>8</v>
+        <f t="shared" si="10"/>
+        <v>-8</v>
       </c>
       <c r="L65" s="5">
         <v>0</v>
@@ -3675,49 +3809,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B66" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="C66" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="D66" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-8</v>
       </c>
       <c r="E66" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-6</v>
       </c>
       <c r="F66" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="G66" s="16">
+        <f t="shared" si="10"/>
+        <v>-2</v>
+      </c>
+      <c r="H66" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I66" s="16">
+        <f t="shared" si="10"/>
         <v>-4</v>
       </c>
-      <c r="G66" s="16">
-        <f t="shared" si="12"/>
+      <c r="J66" s="16">
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
-      <c r="H66" s="16">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="I66" s="16">
-        <f t="shared" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="J66" s="16">
-        <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
       <c r="K66" s="16">
-        <f t="shared" si="12"/>
-        <v>6</v>
+        <f t="shared" si="10"/>
+        <v>-4</v>
       </c>
       <c r="L66" s="16">
         <v>0</v>
@@ -3731,44 +3865,44 @@
         <v>25</v>
       </c>
       <c r="B67" s="16">
-        <f t="shared" si="12"/>
-        <v>6</v>
+        <f t="shared" si="10"/>
+        <v>-6</v>
       </c>
       <c r="C67" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="D67" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="E67" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-8</v>
       </c>
       <c r="F67" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-6</v>
       </c>
       <c r="G67" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>-4</v>
       </c>
       <c r="H67" s="16">
-        <f t="shared" si="12"/>
-        <v>-2</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
       <c r="I67" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J67" s="16">
-        <f t="shared" si="12"/>
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>8</v>
       </c>
       <c r="K67" s="16">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>-10</v>
       </c>
       <c r="L67" s="5">
         <v>0</v>
@@ -3782,44 +3916,44 @@
         <v>27</v>
       </c>
       <c r="B68" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="C68" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="D68" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="E68" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>-10</v>
+      </c>
+      <c r="F68" s="16">
+        <f t="shared" si="10"/>
+        <v>-8</v>
+      </c>
+      <c r="G68" s="16">
+        <f t="shared" si="10"/>
+        <v>-6</v>
+      </c>
+      <c r="H68" s="16">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="I68" s="16">
+        <f t="shared" si="10"/>
+        <v>-8</v>
+      </c>
+      <c r="J68" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K68" s="16">
+        <f t="shared" si="10"/>
         <v>10</v>
-      </c>
-      <c r="F68" s="16">
-        <f t="shared" si="12"/>
-        <v>-8</v>
-      </c>
-      <c r="G68" s="16">
-        <f t="shared" si="12"/>
-        <v>-6</v>
-      </c>
-      <c r="H68" s="16">
-        <f t="shared" si="12"/>
-        <v>-4</v>
-      </c>
-      <c r="I68" s="16">
-        <f t="shared" si="12"/>
-        <v>-2</v>
-      </c>
-      <c r="J68" s="16">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="K68" s="16">
-        <f t="shared" si="12"/>
-        <v>2</v>
       </c>
       <c r="L68" s="16">
         <v>0</v>
@@ -3833,43 +3967,43 @@
         <v>48</v>
       </c>
       <c r="B69" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="C69" s="16">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>-8</v>
       </c>
       <c r="D69" s="16">
-        <f t="shared" si="12"/>
-        <v>6</v>
+        <f t="shared" si="10"/>
+        <v>-6</v>
       </c>
       <c r="E69" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="F69" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>-10</v>
+      </c>
+      <c r="G69" s="16">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="H69" s="16">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="I69" s="16">
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="G69" s="16">
-        <f t="shared" si="12"/>
-        <v>-8</v>
-      </c>
-      <c r="H69" s="16">
-        <f t="shared" si="12"/>
-        <v>-6</v>
-      </c>
-      <c r="I69" s="16">
-        <f t="shared" si="12"/>
-        <v>-4</v>
-      </c>
       <c r="J69" s="16">
-        <f t="shared" si="12"/>
-        <v>-2</v>
+        <f t="shared" si="10"/>
+        <v>-10</v>
       </c>
       <c r="K69" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L69" s="5">
@@ -4000,7 +4134,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>12</v>
       </c>
@@ -4009,39 +4143,39 @@
         <v>0</v>
       </c>
       <c r="C74" s="13">
-        <f t="shared" ref="C74:K74" si="13">+C17/4</f>
+        <f t="shared" ref="C74:K74" si="11">+C17/4</f>
         <v>1</v>
       </c>
       <c r="D74" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="E74" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="F74" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="G74" s="13">
-        <f t="shared" si="13"/>
-        <v>5</v>
+        <f t="shared" si="11"/>
+        <v>-5</v>
       </c>
       <c r="H74" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-4</v>
       </c>
       <c r="I74" s="13">
-        <f t="shared" si="13"/>
-        <v>-3</v>
+        <f t="shared" si="11"/>
+        <v>3</v>
       </c>
       <c r="J74" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-2</v>
       </c>
       <c r="K74" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="L74" s="16">
@@ -4056,44 +4190,44 @@
         <v>14</v>
       </c>
       <c r="B75" s="13">
-        <f t="shared" ref="B75:K83" si="14">+B18/4</f>
+        <f t="shared" ref="B75:K83" si="12">+B18/4</f>
         <v>-1</v>
       </c>
       <c r="C75" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="D75" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E75" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="F75" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="G75" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="H75" s="13">
-        <f t="shared" si="14"/>
-        <v>5</v>
+        <f t="shared" si="12"/>
+        <v>-5</v>
       </c>
       <c r="I75" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-4</v>
       </c>
       <c r="J75" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-3</v>
       </c>
       <c r="K75" s="13">
-        <f t="shared" si="14"/>
-        <v>-2</v>
+        <f t="shared" si="12"/>
+        <v>4</v>
       </c>
       <c r="L75" s="5">
         <v>0</v>
@@ -4107,44 +4241,44 @@
         <v>15</v>
       </c>
       <c r="B76" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-2</v>
       </c>
       <c r="C76" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
       <c r="D76" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E76" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="F76" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="G76" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="H76" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="I76" s="13">
-        <f t="shared" si="14"/>
-        <v>5</v>
+        <f t="shared" si="12"/>
+        <v>-5</v>
       </c>
       <c r="J76" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-4</v>
       </c>
       <c r="K76" s="13">
-        <f t="shared" si="14"/>
-        <v>-3</v>
+        <f t="shared" si="12"/>
+        <v>3</v>
       </c>
       <c r="L76" s="16">
         <v>0</v>
@@ -4158,43 +4292,43 @@
         <v>17</v>
       </c>
       <c r="B77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-3</v>
       </c>
       <c r="C77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-2</v>
       </c>
       <c r="D77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
       <c r="E77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G77" s="13">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f t="shared" si="12"/>
+        <v>-2</v>
       </c>
       <c r="H77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="I77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="J77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="K77" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-4</v>
       </c>
       <c r="L77" s="5">
@@ -4209,43 +4343,43 @@
         <v>19</v>
       </c>
       <c r="B78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-4</v>
       </c>
       <c r="C78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-3</v>
       </c>
       <c r="D78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-2</v>
       </c>
       <c r="E78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
       <c r="F78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H78" s="13">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f t="shared" si="12"/>
+        <v>-2</v>
       </c>
       <c r="I78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="J78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="K78" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="L78" s="16">
@@ -4260,44 +4394,44 @@
         <v>21</v>
       </c>
       <c r="B79" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="C79" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-4</v>
       </c>
       <c r="D79" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-3</v>
       </c>
       <c r="E79" s="13">
-        <f t="shared" si="14"/>
-        <v>-2</v>
+        <f t="shared" si="12"/>
+        <v>2</v>
       </c>
       <c r="F79" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
       <c r="G79" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H79" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="I79" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="J79" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K79" s="13">
-        <f t="shared" si="14"/>
-        <v>4</v>
+        <f t="shared" si="12"/>
+        <v>-4</v>
       </c>
       <c r="L79" s="5">
         <v>0</v>
@@ -4306,49 +4440,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B80" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="C80" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="D80" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-4</v>
       </c>
       <c r="E80" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-3</v>
       </c>
       <c r="F80" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="G80" s="13">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="H80" s="13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I80" s="13">
+        <f t="shared" si="12"/>
         <v>-2</v>
       </c>
-      <c r="G80" s="13">
-        <f t="shared" si="14"/>
+      <c r="J80" s="13">
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
-      <c r="H80" s="13">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="I80" s="13">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="J80" s="13">
-        <f t="shared" si="14"/>
-        <v>2</v>
-      </c>
       <c r="K80" s="13">
-        <f t="shared" si="14"/>
-        <v>3</v>
+        <f t="shared" si="12"/>
+        <v>-2</v>
       </c>
       <c r="L80" s="16">
         <v>0</v>
@@ -4362,44 +4496,44 @@
         <v>25</v>
       </c>
       <c r="B81" s="13">
-        <f t="shared" si="14"/>
-        <v>3</v>
+        <f t="shared" si="12"/>
+        <v>-3</v>
       </c>
       <c r="C81" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="D81" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="E81" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-4</v>
       </c>
       <c r="F81" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-3</v>
       </c>
       <c r="G81" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-2</v>
       </c>
       <c r="H81" s="13">
-        <f t="shared" si="14"/>
-        <v>-1</v>
+        <f t="shared" si="12"/>
+        <v>2</v>
       </c>
       <c r="I81" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J81" s="13">
-        <f t="shared" si="14"/>
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>4</v>
       </c>
       <c r="K81" s="13">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f t="shared" si="12"/>
+        <v>-5</v>
       </c>
       <c r="L81" s="5">
         <v>0</v>
@@ -4413,44 +4547,44 @@
         <v>27</v>
       </c>
       <c r="B82" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="C82" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="D82" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="E82" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
+        <v>-5</v>
+      </c>
+      <c r="F82" s="13">
+        <f t="shared" si="12"/>
+        <v>-4</v>
+      </c>
+      <c r="G82" s="13">
+        <f t="shared" si="12"/>
+        <v>-3</v>
+      </c>
+      <c r="H82" s="13">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="I82" s="13">
+        <f t="shared" si="12"/>
+        <v>-4</v>
+      </c>
+      <c r="J82" s="13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K82" s="13">
+        <f t="shared" si="12"/>
         <v>5</v>
-      </c>
-      <c r="F82" s="13">
-        <f t="shared" si="14"/>
-        <v>-4</v>
-      </c>
-      <c r="G82" s="13">
-        <f t="shared" si="14"/>
-        <v>-3</v>
-      </c>
-      <c r="H82" s="13">
-        <f t="shared" si="14"/>
-        <v>-2</v>
-      </c>
-      <c r="I82" s="13">
-        <f t="shared" si="14"/>
-        <v>-1</v>
-      </c>
-      <c r="J82" s="13">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="K82" s="13">
-        <f t="shared" si="14"/>
-        <v>1</v>
       </c>
       <c r="L82" s="16">
         <v>0</v>
@@ -4464,43 +4598,43 @@
         <v>48</v>
       </c>
       <c r="B83" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="C83" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
+        <v>-4</v>
+      </c>
+      <c r="D83" s="13">
+        <f t="shared" si="12"/>
+        <v>-3</v>
+      </c>
+      <c r="E83" s="13">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="F83" s="13">
+        <f t="shared" si="12"/>
+        <v>-5</v>
+      </c>
+      <c r="G83" s="13">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="H83" s="13">
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
-      <c r="D83" s="13">
-        <f t="shared" si="14"/>
-        <v>3</v>
-      </c>
-      <c r="E83" s="13">
-        <f t="shared" si="14"/>
-        <v>4</v>
-      </c>
-      <c r="F83" s="13">
-        <f t="shared" si="14"/>
+      <c r="I83" s="13">
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="G83" s="13">
-        <f t="shared" si="14"/>
-        <v>-4</v>
-      </c>
-      <c r="H83" s="13">
-        <f t="shared" si="14"/>
-        <v>-3</v>
-      </c>
-      <c r="I83" s="13">
-        <f t="shared" si="14"/>
-        <v>-2</v>
-      </c>
       <c r="J83" s="13">
-        <f t="shared" si="14"/>
-        <v>-1</v>
+        <f t="shared" si="12"/>
+        <v>-5</v>
       </c>
       <c r="K83" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L83" s="5">
@@ -4592,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>31</v>
       </c>
@@ -4671,44 +4805,44 @@
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C92" t="str">
-        <f t="shared" ref="C92:K92" si="15">IF(C17 &lt; 0, "Vida J1 " &amp; C17, "Vida J2 -" &amp; C17)</f>
+        <f t="shared" ref="C92:K92" si="13">IF(C17 &lt; 0, "Vida J1 " &amp; C17, "Vida J2 -" &amp; C17)</f>
         <v>Vida J2 -4</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>Vida J2 -8</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>Vida J2 -12</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>Vida J2 -16</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="15"/>
-        <v>Vida J2 -20</v>
+        <f t="shared" si="13"/>
+        <v>Vida J1 -20</v>
       </c>
       <c r="H92" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>Vida J1 -16</v>
       </c>
       <c r="I92" t="str">
-        <f t="shared" si="15"/>
-        <v>Vida J1 -12</v>
+        <f t="shared" si="13"/>
+        <v>Vida J2 -12</v>
       </c>
       <c r="J92" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>Vida J1 -8</v>
       </c>
       <c r="K92" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>Vida J1 -4</v>
       </c>
       <c r="L92" s="1" t="s">
@@ -4723,40 +4857,40 @@
         <v>14</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" ref="B93:K101" si="16">IF(B18 &lt; 0, "Vida J1 " &amp; B18, "Vida J2 -" &amp; B18)</f>
+        <f t="shared" ref="B93:K101" si="14">IF(B18 &lt; 0, "Vida J1 " &amp; B18, "Vida J2 -" &amp; B18)</f>
         <v>Vida J1 -4</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -4</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -8</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -12</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -16</v>
       </c>
       <c r="H93" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -20</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -20</v>
       </c>
       <c r="I93" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -16</v>
       </c>
       <c r="J93" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -12</v>
       </c>
       <c r="K93" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -8</v>
+        <f t="shared" si="14"/>
+        <v>Vida J2 -16</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>51</v>
@@ -4770,40 +4904,40 @@
         <v>15</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -8</v>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -4</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -4</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -8</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -12</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -16</v>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -20</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -20</v>
       </c>
       <c r="J94" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -16</v>
       </c>
       <c r="K94" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -12</v>
+        <f t="shared" si="14"/>
+        <v>Vida J2 -12</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>51</v>
@@ -4817,39 +4951,39 @@
         <v>17</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -12</v>
       </c>
       <c r="C95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -8</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -4</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -4</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -8</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -8</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -12</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -16</v>
       </c>
       <c r="J95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -20</v>
       </c>
       <c r="K95" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -16</v>
       </c>
       <c r="L95" s="1" t="s">
@@ -4864,39 +4998,39 @@
         <v>19</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -16</v>
       </c>
       <c r="C96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -12</v>
       </c>
       <c r="D96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -8</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -4</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -4</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -8</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -8</v>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -12</v>
       </c>
       <c r="J96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -16</v>
       </c>
       <c r="K96" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -20</v>
       </c>
       <c r="L96" s="1" t="s">
@@ -4911,40 +5045,40 @@
         <v>21</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -20</v>
       </c>
       <c r="C97" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -16</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -12</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -8</v>
+        <f t="shared" si="14"/>
+        <v>Vida J2 -8</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -4</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -4</v>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -8</v>
       </c>
       <c r="J97" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -12</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -16</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -16</v>
       </c>
       <c r="L97" s="1" t="s">
         <v>51</v>
@@ -4953,45 +5087,45 @@
         <v>54</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -16</v>
       </c>
       <c r="C98" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -20</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -16</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -12</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
+        <v>Vida J2 -8</v>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J1 -4</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="14"/>
         <v>Vida J1 -8</v>
       </c>
-      <c r="G98" t="str">
-        <f t="shared" si="16"/>
+      <c r="J98" t="str">
+        <f t="shared" si="14"/>
         <v>Vida J1 -4</v>
       </c>
-      <c r="I98" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -4</v>
-      </c>
-      <c r="J98" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -8</v>
-      </c>
       <c r="K98" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -12</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -8</v>
       </c>
       <c r="L98" s="1" t="s">
         <v>51</v>
@@ -5005,40 +5139,40 @@
         <v>25</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -12</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -12</v>
       </c>
       <c r="C99" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -16</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -20</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -16</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -12</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J1 -8</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -4</v>
+        <f t="shared" si="14"/>
+        <v>Vida J2 -8</v>
       </c>
       <c r="J99" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -4</v>
+        <f t="shared" si="14"/>
+        <v>Vida J2 -16</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -8</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -20</v>
       </c>
       <c r="L99" s="1" t="s">
         <v>51</v>
@@ -5052,40 +5186,40 @@
         <v>27</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -8</v>
       </c>
       <c r="C100" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -12</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -16</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -20</v>
+      </c>
+      <c r="F100" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J1 -16</v>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J1 -12</v>
+      </c>
+      <c r="H100" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J2 -4</v>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J1 -16</v>
+      </c>
+      <c r="K100" t="str">
+        <f t="shared" si="14"/>
         <v>Vida J2 -20</v>
-      </c>
-      <c r="F100" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -16</v>
-      </c>
-      <c r="G100" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -12</v>
-      </c>
-      <c r="H100" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -8</v>
-      </c>
-      <c r="I100" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -4</v>
-      </c>
-      <c r="K100" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -4</v>
       </c>
       <c r="L100" s="1" t="s">
         <v>51</v>
@@ -5099,40 +5233,40 @@
         <v>48</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>Vida J2 -4</v>
       </c>
       <c r="C101" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -16</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J1 -12</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J2 -16</v>
+      </c>
+      <c r="F101" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J1 -20</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="14"/>
+        <v>Vida J2 -16</v>
+      </c>
+      <c r="H101" t="str">
+        <f t="shared" si="14"/>
         <v>Vida J2 -8</v>
       </c>
-      <c r="D101" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -12</v>
-      </c>
-      <c r="E101" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J2 -16</v>
-      </c>
-      <c r="F101" t="str">
-        <f t="shared" si="16"/>
+      <c r="I101" t="str">
+        <f t="shared" si="14"/>
         <v>Vida J2 -20</v>
       </c>
-      <c r="G101" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -16</v>
-      </c>
-      <c r="H101" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -12</v>
-      </c>
-      <c r="I101" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -8</v>
-      </c>
       <c r="J101" t="str">
-        <f t="shared" si="16"/>
-        <v>Vida J1 -4</v>
+        <f t="shared" si="14"/>
+        <v>Vida J1 -20</v>
       </c>
       <c r="L101" s="1" t="s">
         <v>51</v>

</xml_diff>